<commit_message>
<LDG-78> Gramatica e classes para validação e execução de scripts
</commit_message>
<xml_diff>
--- a/docs/Planeamento/SPRINT D/US_SprintD.xlsx
+++ b/docs/Planeamento/SPRINT D/US_SprintD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luism\Desktop\lei20_21_s4_2dl_4\docs\Planeamento\SPRINT D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{238C4004-1CF4-43B3-80FE-2C5838F095B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D42CBE3-299B-4B65-AA0B-52E8B4233C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDCDD7A7-A42D-BB49-A3F1-83703FDDB978}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$H$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -285,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +301,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -341,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -390,6 +402,15 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -724,11 +745,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA5B1A8D-0180-0642-B118-F58C3A59AAC7}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -737,14 +758,14 @@
     <col min="2" max="2" width="13.09765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.796875" style="8" customWidth="1"/>
     <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.796875" style="1"/>
-    <col min="6" max="6" width="75.796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.296875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="79.5" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.796875" style="3"/>
+    <col min="5" max="6" width="10.796875" style="1"/>
+    <col min="7" max="7" width="75.796875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="19.296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="79.5" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
         <v>48</v>
       </c>
@@ -760,18 +781,19 @@
       <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="11">
@@ -786,17 +808,18 @@
       <c r="E2" s="1">
         <v>1007</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="20"/>
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>50</v>
       </c>
@@ -812,17 +835,18 @@
       <c r="E3" s="1">
         <v>3003</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>51</v>
       </c>
@@ -838,17 +862,18 @@
       <c r="E4" s="1">
         <v>3023</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="19"/>
+      <c r="G4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>52</v>
       </c>
@@ -864,17 +889,18 @@
       <c r="E5" s="1">
         <v>3031</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="19"/>
+      <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>53</v>
       </c>
@@ -890,17 +916,18 @@
       <c r="E6" s="1">
         <v>3101</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="19"/>
+      <c r="G6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -916,17 +943,18 @@
       <c r="E7" s="1">
         <v>4003</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="19"/>
+      <c r="G7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>53</v>
       </c>
@@ -942,17 +970,18 @@
       <c r="E8" s="1">
         <v>4051</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="19"/>
+      <c r="G8" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>53</v>
       </c>
@@ -968,17 +997,18 @@
       <c r="E9" s="1">
         <v>4052</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="19"/>
+      <c r="G9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="136.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="136.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
@@ -994,17 +1024,17 @@
       <c r="E10" s="1">
         <v>4071</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="I10" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="165" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>56</v>
       </c>
@@ -1020,17 +1050,17 @@
       <c r="E11" s="1">
         <v>4072</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -1046,17 +1076,17 @@
       <c r="E12" s="1">
         <v>5002</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
@@ -1072,17 +1102,17 @@
       <c r="E13" s="1">
         <v>5003</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="100.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
@@ -1098,17 +1128,17 @@
       <c r="E14" s="1">
         <v>9002</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>57</v>
       </c>
@@ -1124,14 +1154,14 @@
       <c r="E15" s="1">
         <v>2013</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>53</v>
       </c>
@@ -1147,17 +1177,18 @@
       <c r="E16" s="1">
         <v>2102</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="19"/>
+      <c r="G16" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -1173,25 +1204,26 @@
       <c r="E17" s="11">
         <v>3051</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11"/>
+      <c r="G17" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H17" xr:uid="{BF8C8512-301D-2D43-8EDD-4BC55BF43399}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H15">
-      <sortCondition ref="G2:G15"/>
+  <autoFilter ref="A1:I17" xr:uid="{BF8C8512-301D-2D43-8EDD-4BC55BF43399}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
+      <sortCondition ref="H2:H15"/>
       <sortCondition ref="B2:B15"/>
       <sortCondition ref="C2:C15"/>
       <sortCondition ref="E2:E15"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
-    <sortCondition ref="G2:G17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I17">
+    <sortCondition ref="H2:H17"/>
     <sortCondition ref="B2:B17"/>
     <sortCondition ref="C2:C17"/>
     <sortCondition ref="E2:E17"/>

</xml_diff>